<commit_message>
ok, these work now
</commit_message>
<xml_diff>
--- a/excel_files/prediction.xlsx
+++ b/excel_files/prediction.xlsx
@@ -212,6 +212,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -234,10 +235,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -543,21 +545,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col style="1" min="1" customWidth="1" max="1" width="9"/>
-    <col style="1" min="2" customWidth="1" max="2" width="16"/>
-    <col style="1" min="3" customWidth="1" max="3" width="12"/>
-    <col style="1" min="4" customWidth="1" max="4" width="20"/>
-    <col style="1" min="5" customWidth="1" max="5" width="12"/>
-    <col style="1" min="6" customWidth="1" max="6" width="20"/>
-    <col style="1" min="7" customWidth="1" max="7" width="12"/>
-    <col style="1" min="8" customWidth="1" max="8" width="16"/>
-    <col style="1" min="9" customWidth="1" max="9" width="14"/>
-    <col style="1" min="10" customWidth="1" max="10" width="14"/>
-    <col style="1" min="11" customWidth="1" max="11" width="9.1"/>
+    <col style="2" min="1" customWidth="1" max="1" width="9"/>
+    <col style="2" min="2" customWidth="1" max="2" width="16"/>
+    <col style="2" min="3" customWidth="1" max="3" width="12"/>
+    <col style="2" min="4" customWidth="1" max="4" width="20"/>
+    <col style="2" min="5" customWidth="1" max="5" width="12"/>
+    <col style="2" min="6" customWidth="1" max="6" width="20"/>
+    <col style="2" min="7" customWidth="1" max="7" width="12"/>
+    <col style="2" min="8" customWidth="1" max="8" width="16"/>
+    <col style="2" min="9" customWidth="1" max="9" width="14"/>
+    <col style="2" min="10" customWidth="1" max="10" width="14"/>
+    <col style="2" min="11" customWidth="1" max="11" width="9.1"/>
   </cols>
   <sheetData>
     <row spans="1:11" r="1">
-      <c t="s" s="1" r="A1">
+      <c t="s" s="3" r="A1">
         <v>47</v>
       </c>
       <c t="s" s="1" r="B1">
@@ -660,10 +662,10 @@
         <v>1.0</v>
       </c>
       <c t="s" r="C4">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c t="s" r="D4">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c t="s" r="E4">
         <v>1</v>
@@ -672,16 +674,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G4">
-        <v>0.4136956193425253</v>
+        <v>0.16869292138104128</v>
       </c>
       <c t="n" r="H4">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c t="n" r="I4">
-        <v>21.46336318789391</v>
+        <v>22.85264717237921</v>
       </c>
       <c t="n" r="J4">
-        <v>17.718047629143687</v>
+        <v>22.902309322916658</v>
       </c>
     </row>
     <row spans="1:11" r="5">
@@ -692,10 +694,10 @@
         <v>1.0</v>
       </c>
       <c t="s" r="C5">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c t="s" r="D5">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c t="s" r="E5">
         <v>1</v>
@@ -704,16 +706,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G5">
-        <v>0.1643589723267562</v>
+        <v>0.4136956193425253</v>
       </c>
       <c t="n" r="H5">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c t="n" r="I5">
-        <v>22.85264717237921</v>
+        <v>21.46336318789391</v>
       </c>
       <c t="n" r="J5">
-        <v>22.902309322916658</v>
+        <v>17.718047629143687</v>
       </c>
     </row>
     <row spans="1:11" r="6">
@@ -1217,7 +1219,7 @@
         <v>50</v>
       </c>
       <c t="n" r="G21">
-        <v>0.45833011586715033</v>
+        <v>0.48499419811858957</v>
       </c>
       <c t="n" r="H21">
         <v>2.0</v>
@@ -1281,10 +1283,10 @@
         <v>50</v>
       </c>
       <c t="n" r="G23">
-        <v>0.5375784838347345</v>
+        <v>0.5931873813354619</v>
       </c>
       <c t="n" r="H23">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c t="n" r="I23">
         <v>28.199202279341144</v>
@@ -1604,7 +1606,7 @@
         <v>0.5682892755515676</v>
       </c>
       <c t="n" r="H33">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c t="n" r="I33">
         <v>23.521190985634853</v>
@@ -1633,10 +1635,10 @@
         <v>53</v>
       </c>
       <c t="n" s="2" r="G34">
-        <v>0.8578168258455559</v>
+        <v>0.8221724753764443</v>
       </c>
       <c t="n" s="2" r="H34">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c t="n" s="2" r="I34">
         <v>30.673148581261017</v>
@@ -1794,7 +1796,7 @@
         <v>50</v>
       </c>
       <c t="n" r="G39">
-        <v>0.7077371306286907</v>
+        <v>0.7042823394492836</v>
       </c>
       <c t="n" r="H39">
         <v>8.0</v>
@@ -1910,10 +1912,10 @@
         <v>3.0</v>
       </c>
       <c t="s" r="C43">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c t="s" r="D43">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c t="s" r="E43">
         <v>7</v>
@@ -1922,16 +1924,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G43">
-        <v>0.8337593812213009</v>
+        <v>0.3960245000451685</v>
       </c>
       <c t="n" r="H43">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c t="n" r="I43">
-        <v>25.700761511760962</v>
+        <v>20.935648469224034</v>
       </c>
       <c t="n" r="J43">
-        <v>19.20212170608188</v>
+        <v>21.293349698338847</v>
       </c>
     </row>
     <row spans="1:11" r="44">
@@ -1942,10 +1944,10 @@
         <v>3.0</v>
       </c>
       <c t="s" r="C44">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c t="s" r="D44">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c t="s" r="E44">
         <v>7</v>
@@ -1954,16 +1956,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G44">
-        <v>0.3960245000451685</v>
+        <v>0.4632555537156042</v>
       </c>
       <c t="n" r="H44">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c t="n" r="I44">
-        <v>20.935648469224034</v>
+        <v>20.02006078413186</v>
       </c>
       <c t="n" r="J44">
-        <v>21.293349698338847</v>
+        <v>22.365046449131977</v>
       </c>
     </row>
     <row spans="1:11" r="45">
@@ -1974,10 +1976,10 @@
         <v>3.0</v>
       </c>
       <c t="s" r="C45">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c t="s" r="D45">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c t="s" r="E45">
         <v>7</v>
@@ -1986,16 +1988,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G45">
-        <v>0.4632555537156042</v>
+        <v>0.9384825211059815</v>
       </c>
       <c t="n" r="H45">
-        <v>3.0</v>
+        <v>16.0</v>
       </c>
       <c t="n" r="I45">
-        <v>20.02006078413186</v>
+        <v>31.18958873018665</v>
       </c>
       <c t="n" r="J45">
-        <v>22.365046449131977</v>
+        <v>14.312449808920316</v>
       </c>
     </row>
     <row spans="1:11" r="46">
@@ -2006,10 +2008,10 @@
         <v>3.0</v>
       </c>
       <c t="s" r="C46">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c t="s" r="D46">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c t="s" r="E46">
         <v>7</v>
@@ -2018,16 +2020,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G46">
-        <v>0.9384825211059815</v>
+        <v>0.4586322406938861</v>
       </c>
       <c t="n" r="H46">
-        <v>16.0</v>
+        <v>2.0</v>
       </c>
       <c t="n" r="I46">
-        <v>31.18958873018665</v>
+        <v>20.61664256674618</v>
       </c>
       <c t="n" r="J46">
-        <v>14.312449808920316</v>
+        <v>23.18610979686278</v>
       </c>
     </row>
     <row spans="1:11" r="47">
@@ -2038,10 +2040,10 @@
         <v>3.0</v>
       </c>
       <c t="s" r="C47">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c t="s" r="D47">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c t="s" r="E47">
         <v>7</v>
@@ -2050,16 +2052,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G47">
-        <v>0.4586322406938861</v>
+        <v>0.8337593812213009</v>
       </c>
       <c t="n" r="H47">
-        <v>2.0</v>
+        <v>13.0</v>
       </c>
       <c t="n" r="I47">
-        <v>20.61664256674618</v>
+        <v>25.700761511760962</v>
       </c>
       <c t="n" r="J47">
-        <v>23.18610979686278</v>
+        <v>19.20212170608188</v>
       </c>
     </row>
     <row spans="1:11" r="48">
@@ -2117,7 +2119,7 @@
         <v>0.8400286816437176</v>
       </c>
       <c t="n" r="H49">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c t="n" r="I49">
         <v>26.712473615338325</v>
@@ -2149,7 +2151,7 @@
         <v>0.7137493962065052</v>
       </c>
       <c t="n" s="2" r="H50">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c t="n" s="2" r="I50">
         <v>24.30400118823409</v>
@@ -2231,10 +2233,10 @@
         <v>4.0</v>
       </c>
       <c t="s" r="C53">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c t="s" r="D53">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c t="s" r="E53">
         <v>10</v>
@@ -2243,16 +2245,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G53">
-        <v>0.26477635992814785</v>
+        <v>0.3370473791308303</v>
       </c>
       <c t="n" r="H53">
         <v>2.0</v>
       </c>
       <c t="n" r="I53">
-        <v>21.00597421738928</v>
+        <v>23.82140513425579</v>
       </c>
       <c t="n" r="J53">
-        <v>22.387996445394954</v>
+        <v>16.05815278016444</v>
       </c>
     </row>
     <row spans="1:11" r="54">
@@ -2263,10 +2265,10 @@
         <v>4.0</v>
       </c>
       <c t="s" r="C54">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c t="s" r="D54">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c t="s" r="E54">
         <v>10</v>
@@ -2275,16 +2277,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G54">
-        <v>0.3370473791308303</v>
+        <v>0.38236218434747193</v>
       </c>
       <c t="n" r="H54">
         <v>3.0</v>
       </c>
       <c t="n" r="I54">
-        <v>23.82140513425579</v>
+        <v>21.00597421738928</v>
       </c>
       <c t="n" r="J54">
-        <v>16.05815278016444</v>
+        <v>22.387996445394954</v>
       </c>
     </row>
     <row spans="1:11" r="55">
@@ -2423,10 +2425,10 @@
         <v>4.0</v>
       </c>
       <c t="s" r="C59">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c t="s" r="D59">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c t="s" r="E59">
         <v>10</v>
@@ -2435,16 +2437,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G59">
-        <v>0.7466160516611761</v>
+        <v>0.6867209160678648</v>
       </c>
       <c t="n" r="H59">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c t="n" r="I59">
-        <v>23.713558019927895</v>
+        <v>28.387801952204313</v>
       </c>
       <c t="n" r="J59">
-        <v>26.159080215571187</v>
+        <v>24.29278645694332</v>
       </c>
     </row>
     <row spans="1:11" r="60">
@@ -2455,10 +2457,10 @@
         <v>4.0</v>
       </c>
       <c t="s" r="C60">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c t="s" r="D60">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c t="s" r="E60">
         <v>10</v>
@@ -2467,16 +2469,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G60">
-        <v>0.752532581537048</v>
+        <v>0.7466160516611761</v>
       </c>
       <c t="n" r="H60">
         <v>10.0</v>
       </c>
       <c t="n" r="I60">
-        <v>25.127714394165153</v>
+        <v>23.713558019927895</v>
       </c>
       <c t="n" r="J60">
-        <v>15.899967955699596</v>
+        <v>26.159080215571187</v>
       </c>
     </row>
     <row spans="1:11" r="61">
@@ -2487,10 +2489,10 @@
         <v>4.0</v>
       </c>
       <c t="s" r="C61">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c t="s" r="D61">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c t="s" r="E61">
         <v>10</v>
@@ -2499,16 +2501,16 @@
         <v>50</v>
       </c>
       <c t="n" r="G61">
-        <v>0.7605285874774715</v>
+        <v>0.752532581537048</v>
       </c>
       <c t="n" r="H61">
         <v>11.0</v>
       </c>
       <c t="n" r="I61">
-        <v>28.387801952204313</v>
+        <v>25.127714394165153</v>
       </c>
       <c t="n" r="J61">
-        <v>24.29278645694332</v>
+        <v>15.899967955699596</v>
       </c>
     </row>
     <row spans="1:11" r="62">

</xml_diff>